<commit_message>
Day 4 part 1
☠️
</commit_message>
<xml_diff>
--- a/Felix/Day3/24d3p2.xlsx
+++ b/Felix/Day3/24d3p2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b58bf48a7331aef/Documents/AdventOfCode/aoc24/Felix/Day3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{27E87C23-7C6F-4BB4-97F1-66218E16C50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77F7CE3B-1240-4A03-B977-E751C23C6C39}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{27E87C23-7C6F-4BB4-97F1-66218E16C50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC7B493F-E714-4CB8-B77D-FCDFCC7DAA9C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9BC4DD3-9E69-4E94-82BB-889EE700334F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9BC4DD3-9E69-4E94-82BB-889EE700334F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,8 @@
   </environmentDefinition>
   <pythonScripts>
     <pythonScript>
-      <code xml:space="preserve">import re
-re.findall("mul\(\d+,\d+\)|do\(\)|don't\(\)",xl(%P2%))
-</code>
+      <code>import re
+re.findall("mul\(\d+,\d+\)|do\(\)|don't\(\)",xl(%P2%))</code>
     </pythonScript>
   </pythonScripts>
 </python>
@@ -492,7 +491,7 @@
   <dimension ref="A1:J725"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>